<commit_message>
Initial commit: ProfitFirst affiliate platform with Excel storage
</commit_message>
<xml_diff>
--- a/server/data/signups.xlsx
+++ b/server/data/signups.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>Timestamp</t>
   </si>
@@ -68,6 +68,36 @@
   </si>
   <si>
     <t>$2a$10$BsQfB91TJ7pWVJz1b9HgROGP5xkAMI5EkK.8HWsN1fHr/LOhBgfSi</t>
+  </si>
+  <si>
+    <t>2025-10-26T09:48:47.915Z</t>
+  </si>
+  <si>
+    <t>Test User</t>
+  </si>
+  <si>
+    <t>test@example.com</t>
+  </si>
+  <si>
+    <t>testuser123</t>
+  </si>
+  <si>
+    <t>password123</t>
+  </si>
+  <si>
+    <t>2025-10-26T09:49:40.649Z</t>
+  </si>
+  <si>
+    <t>Harsh Chandrakant Mali</t>
+  </si>
+  <si>
+    <t>jyxuta@cyclelove.cc</t>
+  </si>
+  <si>
+    <t>Q23n1sdjk</t>
+  </si>
+  <si>
+    <t>qwe123decdcs</t>
   </si>
 </sst>
 </file>
@@ -468,7 +498,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
@@ -559,6 +589,52 @@
         <v>15</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Fix: Standardize border radius to 12px, optimize FAQ animations, fix scrollbar issues, and integrate Google Sheets
</commit_message>
<xml_diff>
--- a/server/data/signups.xlsx
+++ b/server/data/signups.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>Timestamp</t>
   </si>
@@ -98,6 +98,21 @@
   </si>
   <si>
     <t>qwe123decdcs</t>
+  </si>
+  <si>
+    <t>2025-10-27T11:02:02.845Z</t>
+  </si>
+  <si>
+    <t>Patrick Sharma</t>
+  </si>
+  <si>
+    <t>patricksharma1234@gmail.com</t>
+  </si>
+  <si>
+    <t>Ca23m6Na</t>
+  </si>
+  <si>
+    <t>HBhjbs234</t>
   </si>
 </sst>
 </file>
@@ -498,7 +513,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
@@ -635,6 +650,29 @@
         <v>13</v>
       </c>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>